<commit_message>
Added all SQLite related stuff
</commit_message>
<xml_diff>
--- a/src/test/resources/org/nexial/core/utils/script_good.xlsx
+++ b/src/test/resources/org/nexial/core/utils/script_good.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10305"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/ep/sentry/sentry-core/src/test/resources/com/ep/qa/sentry/utils/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/org/nexial/core/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr documentId="13_ncr:1_{43814563-ABCD-A04B-981D-9950544EFB78}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32"/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="1" tabRatio="500" windowHeight="15720" windowWidth="51200" xWindow="0" yWindow="16200"/>
+    <workbookView activeTab="1" tabRatio="500" windowHeight="15720" windowWidth="33600" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="5200" firstSheet="1"/>
   </bookViews>
   <sheets>
     <sheet name="#system" r:id="rId1" sheetId="4" state="hidden"/>
     <sheet name="Test Scenrio" r:id="rId2" sheetId="2"/>
   </sheets>
   <definedNames>
+    <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
     <definedName name="base">'#system'!$C$2:$C$31</definedName>
+    <definedName name="csv">'#system'!$D$2:$D$4</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
     <definedName name="desktop">'#system'!$E$2:$E$91</definedName>
@@ -24,24 +27,24 @@
     <definedName name="external">'#system'!$G$2:$G$3</definedName>
     <definedName name="image">'#system'!$H$2:$H$5</definedName>
     <definedName name="io">'#system'!$I$2:$I$21</definedName>
+    <definedName name="jms">'#system'!$J$2:$J$4</definedName>
     <definedName name="json">'#system'!$K$2:$K$11</definedName>
+    <definedName name="mail">'#system'!$L$2:$L$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
-    <definedName name="target">'#system'!$A$2:$A$21</definedName>
-    <definedName name="xml">'#system'!$U$2:$U$11</definedName>
-    <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
-    <definedName name="csv">'#system'!$D$2:$D$4</definedName>
-    <definedName name="jms">'#system'!$J$2:$J$4</definedName>
-    <definedName name="mail">'#system'!$L$2:$L$2</definedName>
     <definedName name="number">'#system'!$M$2:$M$14</definedName>
     <definedName name="pdf">'#system'!$N$2:$N$16</definedName>
     <definedName name="rdbms">'#system'!$O$2:$O$6</definedName>
-    <definedName name="ssh">'#system'!$P$2:$P$9</definedName>
-    <definedName name="web">'#system'!$Q$2:$Q$108</definedName>
-    <definedName name="webalert">'#system'!$R$2:$R$6</definedName>
-    <definedName name="webcookie">'#system'!$S$2:$S$8</definedName>
-    <definedName name="ws">'#system'!$T$2:$T$16</definedName>
+    <definedName name="ssh">'#system'!$Q$2:$Q$9</definedName>
+    <definedName name="target">'#system'!$A$2:$A$23</definedName>
+    <definedName name="web">'#system'!$S$2:$S$108</definedName>
+    <definedName name="webalert">'#system'!$T$2:$T$6</definedName>
+    <definedName name="webcookie">'#system'!$U$2:$U$8</definedName>
+    <definedName name="ws">'#system'!$V$2:$V$16</definedName>
+    <definedName name="xml">'#system'!$W$2:$W$11</definedName>
+    <definedName name="redis">'#system'!$P$2:$P$10</definedName>
+    <definedName name="step">'#system'!$R$2:$R$4</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -54,13 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="526">
-  <si>
-    <t>jira</t>
-  </si>
-  <si>
-    <t>zephyr</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="428">
   <si>
     <t>description</t>
   </si>
@@ -95,9 +92,6 @@
     <t>execution summary</t>
   </si>
   <si>
-    <t>test case</t>
-  </si>
-  <si>
     <t>project</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
     <t>base</t>
   </si>
   <si>
-    <t>db</t>
-  </si>
-  <si>
     <t>io</t>
   </si>
   <si>
@@ -134,9 +125,6 @@
     <t>release</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>desktop</t>
   </si>
   <si>
@@ -152,30 +140,6 @@
     <t>json</t>
   </si>
   <si>
-    <t>math</t>
-  </si>
-  <si>
-    <t>runJavaMain(class)</t>
-  </si>
-  <si>
-    <t>addHour(date,hour,var)</t>
-  </si>
-  <si>
-    <t>runFile(connection,file,var,trans)</t>
-  </si>
-  <si>
-    <t>assertCheck(widget)</t>
-  </si>
-  <si>
-    <t>read(file,worksheet,range,var)</t>
-  </si>
-  <si>
-    <t>crop(image,xy,width,height,saveTo)</t>
-  </si>
-  <si>
-    <t>assertEqual(file1,file2)</t>
-  </si>
-  <si>
     <t>assertElementCount(json,jsonpath,count)</t>
   </si>
   <si>
@@ -185,318 +149,69 @@
     <t>assertContains(text,substring)</t>
   </si>
   <si>
-    <t>addMinute(date,minute,var)</t>
-  </si>
-  <si>
-    <t>runSQL(connection,sql,var)</t>
-  </si>
-  <si>
-    <t>assertDisabled(widget)</t>
-  </si>
-  <si>
-    <t>toXLSX(xls,xlsx)</t>
-  </si>
-  <si>
     <t>runProgram(programPathAndParms)</t>
   </si>
   <si>
     <t>resize(image,width,height,saveTo)</t>
   </si>
   <si>
-    <t>assertNotEqual(file1,file2)</t>
-  </si>
-  <si>
     <t>assertElementPresent(json,jsonpath)</t>
   </si>
   <si>
     <t>assertGreaterOrEqual(num1,num2)</t>
   </si>
   <si>
-    <t>assertCount(text,regex,expected)</t>
-  </si>
-  <si>
-    <t>addMonth(date,month,var)</t>
-  </si>
-  <si>
-    <t>runSQLs(connection,sqls,var,trans)</t>
-  </si>
-  <si>
-    <t>assertEnabled(widget)</t>
-  </si>
-  <si>
-    <t>write(file,worksheet,startCell,var)</t>
-  </si>
-  <si>
-    <t>assertSame(baseline,subject,failFast)</t>
-  </si>
-  <si>
-    <t>assertSame(expected,actual)</t>
-  </si>
-  <si>
     <t>assertLesser(num1,num2)</t>
   </si>
   <si>
     <t>assertEndsWith(text,suffix)</t>
   </si>
   <si>
-    <t>addSecond(date,second,var)</t>
-  </si>
-  <si>
-    <t>assertGridCellsPresent(grid,cells,inOrder)</t>
-  </si>
-  <si>
-    <t>compareCSV(baseline,subject,failFast)</t>
-  </si>
-  <si>
-    <t>assertValid(json,schema)</t>
-  </si>
-  <si>
     <t>assertLesserOrEqual(num1,num2)</t>
   </si>
   <si>
-    <t>assertEqual(value1,value2)</t>
-  </si>
-  <si>
-    <t>addWeek(date,week,var)</t>
-  </si>
-  <si>
-    <t>assertGridColumnPresent(grid,column,arrays,inOrder)</t>
-  </si>
-  <si>
-    <t>compareImages(baseline,test)</t>
-  </si>
-  <si>
     <t>assertValue(json,jsonpath,expected)</t>
   </si>
   <si>
-    <t>average(array)</t>
-  </si>
-  <si>
-    <t>assertMatch(text,regex)</t>
-  </si>
-  <si>
-    <t>addYear(date,year,var)</t>
-  </si>
-  <si>
-    <t>assertGridHeadersPresent(grid,headers)</t>
-  </si>
-  <si>
     <t>assertValues(json,jsonpath,array,exactOrder)</t>
   </si>
   <si>
-    <t>calculate(formula,var)</t>
-  </si>
-  <si>
-    <t>assertNotEqual(value1,value2)</t>
-  </si>
-  <si>
-    <t>assertDaysApart(date1,date2,expected)</t>
-  </si>
-  <si>
-    <t>assertPresent(widget,type)</t>
-  </si>
-  <si>
-    <t>count(basePath,filePattern,var)</t>
-  </si>
-  <si>
     <t>assertWellformed(json)</t>
   </si>
   <si>
-    <t>ceiling(value,var)</t>
-  </si>
-  <si>
     <t>assertStartsWith(text,prefix)</t>
   </si>
   <si>
-    <t>assertNewer(date1,date2,format)</t>
-  </si>
-  <si>
-    <t>assertSelected(widget,text)</t>
-  </si>
-  <si>
     <t>deleteFiles(location,recursive)</t>
   </si>
   <si>
-    <t>readFile(file,var)</t>
-  </si>
-  <si>
-    <t>floor(value,var)</t>
-  </si>
-  <si>
-    <t>assertTextOrder(text,descending)</t>
-  </si>
-  <si>
-    <t>assertOlder(date1,date2,format)</t>
-  </si>
-  <si>
-    <t>assertSelectedMulti(widget,array)</t>
-  </si>
-  <si>
-    <t>excelToCSV(excel,worksheet,csvFile)</t>
-  </si>
-  <si>
     <t>storeCount(json,jsonpath,var)</t>
   </si>
   <si>
-    <t>max(array)</t>
-  </si>
-  <si>
-    <t>fail(reason)</t>
-  </si>
-  <si>
-    <t>convertFormat(date,from,to,var)</t>
-  </si>
-  <si>
-    <t>assertText(widget,expected)</t>
-  </si>
-  <si>
     <t>storeValue(json,jsonpath,var)</t>
   </si>
   <si>
-    <t>min(array)</t>
-  </si>
-  <si>
     <t>increment(var,amount)</t>
   </si>
   <si>
-    <t>toGMT(date1,format)</t>
-  </si>
-  <si>
-    <t>assertUncheck(widget)</t>
-  </si>
-  <si>
     <t>moveFiles(source,target)</t>
   </si>
   <si>
     <t>storeValues(json,jsonpath,var)</t>
   </si>
   <si>
-    <t>round(value,closestDigit,var)</t>
-  </si>
-  <si>
-    <t>incrementChar(var,amount,type)</t>
-  </si>
-  <si>
-    <t>toTime(date,format,var)</t>
-  </si>
-  <si>
-    <t>check(widget)</t>
-  </si>
-  <si>
-    <t>readProperty(file,property,var)</t>
-  </si>
-  <si>
-    <t>writeFile(var,file)</t>
-  </si>
-  <si>
-    <t>log(text)</t>
-  </si>
-  <si>
-    <t>clickButton(label)</t>
-  </si>
-  <si>
-    <t>readText(file,var)</t>
-  </si>
-  <si>
-    <t>mergeAfter(var,targetVar)</t>
-  </si>
-  <si>
-    <t>clickTextbox(widget)</t>
-  </si>
-  <si>
-    <t>saveFileInfo(file,var)</t>
-  </si>
-  <si>
-    <t>mergeBefore(var,targetVar)</t>
-  </si>
-  <si>
-    <t>enter()</t>
-  </si>
-  <si>
     <t>unzip(zipFile,target)</t>
   </si>
   <si>
-    <t>prependToVar(var,text)</t>
-  </si>
-  <si>
-    <t>mouseMove(x,y)</t>
-  </si>
-  <si>
     <t>writeProperty(file,property,value)</t>
   </si>
   <si>
-    <t>removeVar(var)</t>
-  </si>
-  <si>
-    <t>saveGridData(grid,var)</t>
-  </si>
-  <si>
-    <t>writeText(file,content,append)</t>
-  </si>
-  <si>
-    <t>replaceAndSave(text,regex,replace,var)</t>
-  </si>
-  <si>
-    <t>saveGridHeader(grid,var)</t>
-  </si>
-  <si>
     <t>zip(filePattern,zipFile)</t>
   </si>
   <si>
-    <t>saveMatches(text,regex,var)</t>
-  </si>
-  <si>
-    <t>saveSelected(widget,var)</t>
-  </si>
-  <si>
-    <t>saveToVar(value,var)</t>
-  </si>
-  <si>
-    <t>saveText(widget,var)</t>
-  </si>
-  <si>
-    <t>split(text,delim,var)</t>
-  </si>
-  <si>
-    <t>select(widget,text)</t>
-  </si>
-  <si>
-    <t>startVideo()</t>
-  </si>
-  <si>
-    <t>selectDate(widget,date)</t>
-  </si>
-  <si>
-    <t>stopVideo()</t>
-  </si>
-  <si>
-    <t>selectMulti(widget,array)</t>
-  </si>
-  <si>
-    <t>substringAfter(text,delim,var)</t>
-  </si>
-  <si>
-    <t>tab()</t>
-  </si>
-  <si>
-    <t>substringBefore(text,delim,var)</t>
-  </si>
-  <si>
-    <t>tabBack()</t>
-  </si>
-  <si>
-    <t>substringBetween(text,start,end,var)</t>
-  </si>
-  <si>
-    <t>type(widget,text,modifier)</t>
-  </si>
-  <si>
     <t>wait(waitMs)</t>
   </si>
   <si>
-    <t>uncheck(widget)</t>
-  </si>
-  <si>
     <t>Test Case #1</t>
   </si>
   <si>
@@ -506,72 +221,9 @@
     <t>description of test step #2</t>
   </si>
   <si>
-    <t>xml.assertElementAbsent(xml,xpath)</t>
-  </si>
-  <si>
-    <t>xml.assertElementCount(xml,xpath,count)</t>
-  </si>
-  <si>
-    <t>xml.assertElementPresent(xml,xpath)</t>
-  </si>
-  <si>
-    <t>xml.assertValue(xml,xpath,expected)</t>
-  </si>
-  <si>
-    <t>xml.assertValues(xml,xpath,array,exactOrder)</t>
-  </si>
-  <si>
-    <t>xml.assertWellformed(xml)</t>
-  </si>
-  <si>
-    <t>xml.smartCreate(config)</t>
-  </si>
-  <si>
-    <t>xml.storeCount(xml,xpath,var)</t>
-  </si>
-  <si>
-    <t>xml.storeValue(xml,xpath,var)</t>
-  </si>
-  <si>
-    <t>xml.storeValues(xml,xpath,var)</t>
-  </si>
-  <si>
-    <t>scope(name,mapping)</t>
-  </si>
-  <si>
-    <t>appendToVar(var,text)</t>
-  </si>
-  <si>
-    <t>addDay(date,day,var)</t>
-  </si>
-  <si>
-    <t>resultToCSV(var,csvFile,delim,header)</t>
-  </si>
-  <si>
-    <t>assertActivewidget(expected)</t>
-  </si>
-  <si>
     <t>clear(file,worksheet,range)</t>
   </si>
   <si>
-    <t>runJUnit(class)</t>
-  </si>
-  <si>
-    <t>convert(image,format,var)</t>
-  </si>
-  <si>
-    <t>assertDifferent(baselinePath,currentPath)</t>
-  </si>
-  <si>
-    <t>assertElementAbsent(json,jsonpath)</t>
-  </si>
-  <si>
-    <t>assertEqual(num1,num2)</t>
-  </si>
-  <si>
-    <t>xml.assertCorrectness(xml,schema)</t>
-  </si>
-  <si>
     <t>Hello World!</t>
   </si>
   <si>
@@ -1632,14 +1284,71 @@
   </si>
   <si>
     <t>cmd type</t>
+  </si>
+  <si>
+    <t>story / feature</t>
+  </si>
+  <si>
+    <t>test id</t>
+  </si>
+  <si>
+    <t>redis</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>saveRowCount(var)</t>
+  </si>
+  <si>
+    <t>saveTableRowsRange(var,beginRow,endRow)</t>
+  </si>
+  <si>
+    <t>assertBetween(num,min,max)</t>
+  </si>
+  <si>
+    <t>append(profile,key,value)</t>
+  </si>
+  <si>
+    <t>assertKeyExists(profile,key)</t>
+  </si>
+  <si>
+    <t>delete(profile,key)</t>
+  </si>
+  <si>
+    <t>flushAll(profile)</t>
+  </si>
+  <si>
+    <t>flushDb(profile)</t>
+  </si>
+  <si>
+    <t>rename(profile,current,new)</t>
+  </si>
+  <si>
+    <t>set(profile,key,value)</t>
+  </si>
+  <si>
+    <t>store(var,profile,key)</t>
+  </si>
+  <si>
+    <t>storeKeys(var,profile,keyPattern)</t>
+  </si>
+  <si>
+    <t>observe(prompt)</t>
+  </si>
+  <si>
+    <t>perform(instructions)</t>
+  </si>
+  <si>
+    <t>validate(prompt,responses,passResponses)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1786,84 +1495,8 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="3E511F"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="287389"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="5A5A32"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="11.0"/>
-      <color rgb="12284A"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="0000FF"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="006100"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="808080"/>
-      <u val="none"/>
-    </font>
   </fonts>
-  <fills count="46">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2001,127 +1634,8 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFF"/>
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF"/>
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="48">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -2406,200 +1920,6 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C8B4B4"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C8B4B4"/>
-      </left>
-      <right style="thin">
-        <color rgb="C8B4B4"/>
-      </right>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="DCDCDC"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="DCDCDC"/>
-      </left>
-      <right style="thin">
-        <color rgb="DCDCDC"/>
-      </right>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDCDCD"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDCDCD"/>
-      </left>
-      <right style="thin">
-        <color rgb="CDCDCD"/>
-      </right>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C3C3C3"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C3C3C3"/>
-      </left>
-      <right style="thin">
-        <color rgb="C3C3C3"/>
-      </right>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -2607,7 +1927,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="47">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="3" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -2697,12 +2017,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="5" fillId="3" fontId="5" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -2717,6 +2031,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="5" fillId="3" fontId="6" numFmtId="49" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -2727,76 +2047,40 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="15" fillId="6" fontId="11" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="15" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="9" fontId="13" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="19" fillId="12" fontId="15" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="19" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="23" fillId="15" fontId="16" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="23" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="27" fillId="18" fontId="17" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="27" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="27" fillId="18" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="27" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="21" fontId="19" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="24" fontId="20" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="21" fontId="21" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="35" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="39" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="36" borderId="43" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="39" borderId="47" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="39" borderId="47" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="42" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="45" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="42" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2869,6 +2153,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3136,10 +2423,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V108"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X108"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" tabSelected="false">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -3150,1430 +2437,1478 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>183</v>
+        <v>66</v>
       </c>
       <c r="K1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>184</v>
+        <v>67</v>
       </c>
       <c r="M1" t="s">
-        <v>185</v>
+        <v>68</v>
       </c>
       <c r="N1" t="s">
-        <v>186</v>
+        <v>69</v>
       </c>
       <c r="O1" t="s">
-        <v>187</v>
+        <v>70</v>
       </c>
       <c r="P1" t="s">
-        <v>188</v>
+        <v>411</v>
       </c>
       <c r="Q1" t="s">
-        <v>189</v>
+        <v>71</v>
       </c>
       <c r="R1" t="s">
-        <v>190</v>
+        <v>412</v>
       </c>
       <c r="S1" t="s">
-        <v>191</v>
+        <v>72</v>
       </c>
       <c r="T1" t="s">
-        <v>192</v>
+        <v>73</v>
       </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>74</v>
+      </c>
+      <c r="V1" t="s">
+        <v>75</v>
+      </c>
+      <c r="W1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>227</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
-        <v>230</v>
+        <v>113</v>
       </c>
       <c r="F2" t="s">
-        <v>165</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>326</v>
+        <v>209</v>
       </c>
       <c r="H2" t="s">
-        <v>327</v>
+        <v>210</v>
       </c>
       <c r="I2" t="s">
-        <v>204</v>
+        <v>87</v>
       </c>
       <c r="J2" t="s">
-        <v>340</v>
+        <v>223</v>
       </c>
       <c r="K2" t="s">
-        <v>343</v>
+        <v>226</v>
       </c>
       <c r="L2" t="s">
-        <v>345</v>
+        <v>228</v>
       </c>
       <c r="M2" t="s">
-        <v>346</v>
+        <v>415</v>
       </c>
       <c r="N2" t="s">
-        <v>353</v>
+        <v>236</v>
       </c>
       <c r="O2" t="s">
-        <v>368</v>
+        <v>251</v>
       </c>
       <c r="P2" t="s">
-        <v>373</v>
+        <v>416</v>
       </c>
       <c r="Q2" t="s">
-        <v>381</v>
+        <v>256</v>
       </c>
       <c r="R2" t="s">
-        <v>487</v>
+        <v>425</v>
       </c>
       <c r="S2" t="s">
-        <v>492</v>
+        <v>264</v>
       </c>
       <c r="T2" t="s">
-        <v>499</v>
+        <v>370</v>
       </c>
       <c r="U2" t="s">
-        <v>514</v>
+        <v>375</v>
+      </c>
+      <c r="V2" t="s">
+        <v>382</v>
+      </c>
+      <c r="W2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
       <c r="D3" t="s">
-        <v>228</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>231</v>
+        <v>114</v>
       </c>
       <c r="F3" t="s">
-        <v>320</v>
+        <v>203</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>328</v>
+        <v>211</v>
       </c>
       <c r="I3" t="s">
-        <v>207</v>
+        <v>90</v>
       </c>
       <c r="J3" t="s">
-        <v>341</v>
+        <v>224</v>
       </c>
       <c r="K3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="M3" t="s">
-        <v>204</v>
+        <v>87</v>
       </c>
       <c r="N3" t="s">
-        <v>354</v>
+        <v>237</v>
       </c>
       <c r="O3" t="s">
-        <v>369</v>
+        <v>252</v>
       </c>
       <c r="P3" t="s">
-        <v>374</v>
+        <v>417</v>
       </c>
       <c r="Q3" t="s">
-        <v>382</v>
+        <v>257</v>
       </c>
       <c r="R3" t="s">
-        <v>488</v>
+        <v>426</v>
       </c>
       <c r="S3" t="s">
-        <v>493</v>
+        <v>265</v>
       </c>
       <c r="T3" t="s">
-        <v>500</v>
+        <v>371</v>
       </c>
       <c r="U3" t="s">
-        <v>515</v>
+        <v>376</v>
+      </c>
+      <c r="V3" t="s">
+        <v>383</v>
+      </c>
+      <c r="W3" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>112</v>
       </c>
       <c r="E4" t="s">
-        <v>232</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
-        <v>321</v>
+        <v>204</v>
       </c>
       <c r="H4" t="s">
-        <v>329</v>
+        <v>212</v>
       </c>
       <c r="I4" t="s">
-        <v>330</v>
+        <v>213</v>
       </c>
       <c r="J4" t="s">
-        <v>342</v>
+        <v>225</v>
       </c>
       <c r="K4" t="s">
-        <v>344</v>
+        <v>227</v>
       </c>
       <c r="M4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="N4" t="s">
-        <v>355</v>
+        <v>238</v>
       </c>
       <c r="O4" t="s">
-        <v>370</v>
+        <v>253</v>
       </c>
       <c r="P4" t="s">
-        <v>375</v>
+        <v>418</v>
       </c>
       <c r="Q4" t="s">
-        <v>383</v>
+        <v>258</v>
       </c>
       <c r="R4" t="s">
-        <v>489</v>
+        <v>427</v>
       </c>
       <c r="S4" t="s">
-        <v>494</v>
+        <v>266</v>
       </c>
       <c r="T4" t="s">
-        <v>501</v>
+        <v>372</v>
       </c>
       <c r="U4" t="s">
-        <v>516</v>
+        <v>377</v>
+      </c>
+      <c r="V4" t="s">
+        <v>384</v>
+      </c>
+      <c r="W4" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>85</v>
       </c>
       <c r="E5" t="s">
-        <v>233</v>
+        <v>116</v>
       </c>
       <c r="F5" t="s">
-        <v>322</v>
+        <v>205</v>
       </c>
       <c r="H5" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>227</v>
+        <v>110</v>
       </c>
       <c r="K5" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="M5" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="N5" t="s">
-        <v>356</v>
+        <v>239</v>
       </c>
       <c r="O5" t="s">
-        <v>371</v>
+        <v>254</v>
       </c>
       <c r="P5" t="s">
-        <v>376</v>
+        <v>419</v>
       </c>
       <c r="Q5" t="s">
-        <v>384</v>
-      </c>
-      <c r="R5" t="s">
-        <v>490</v>
+        <v>259</v>
       </c>
       <c r="S5" t="s">
-        <v>495</v>
+        <v>267</v>
       </c>
       <c r="T5" t="s">
-        <v>502</v>
+        <v>373</v>
       </c>
       <c r="U5" t="s">
-        <v>517</v>
+        <v>378</v>
+      </c>
+      <c r="V5" t="s">
+        <v>385</v>
+      </c>
+      <c r="W5" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>203</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
-        <v>234</v>
+        <v>117</v>
       </c>
       <c r="F6" t="s">
-        <v>323</v>
+        <v>206</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K6" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="M6" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="N6" t="s">
-        <v>357</v>
+        <v>240</v>
       </c>
       <c r="O6" t="s">
-        <v>372</v>
+        <v>255</v>
       </c>
       <c r="P6" t="s">
-        <v>377</v>
+        <v>420</v>
       </c>
       <c r="Q6" t="s">
-        <v>385</v>
-      </c>
-      <c r="R6" t="s">
-        <v>491</v>
+        <v>260</v>
       </c>
       <c r="S6" t="s">
-        <v>496</v>
+        <v>268</v>
       </c>
       <c r="T6" t="s">
-        <v>503</v>
+        <v>374</v>
       </c>
       <c r="U6" t="s">
-        <v>518</v>
+        <v>379</v>
+      </c>
+      <c r="V6" t="s">
+        <v>386</v>
+      </c>
+      <c r="W6" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>235</v>
+        <v>118</v>
       </c>
       <c r="F7" t="s">
-        <v>324</v>
+        <v>207</v>
       </c>
       <c r="I7" t="s">
-        <v>331</v>
+        <v>214</v>
       </c>
       <c r="K7" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="M7" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="N7" t="s">
-        <v>358</v>
+        <v>241</v>
       </c>
       <c r="P7" t="s">
-        <v>378</v>
+        <v>421</v>
       </c>
       <c r="Q7" t="s">
-        <v>386</v>
+        <v>261</v>
       </c>
       <c r="S7" t="s">
-        <v>497</v>
-      </c>
-      <c r="T7" t="s">
-        <v>504</v>
+        <v>269</v>
       </c>
       <c r="U7" t="s">
-        <v>519</v>
+        <v>380</v>
+      </c>
+      <c r="V7" t="s">
+        <v>387</v>
+      </c>
+      <c r="W7" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>204</v>
+        <v>87</v>
       </c>
       <c r="E8" t="s">
-        <v>236</v>
+        <v>119</v>
       </c>
       <c r="F8" t="s">
-        <v>325</v>
+        <v>208</v>
       </c>
       <c r="I8" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="K8" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="M8" t="s">
-        <v>347</v>
+        <v>230</v>
       </c>
       <c r="N8" t="s">
-        <v>359</v>
+        <v>242</v>
       </c>
       <c r="P8" t="s">
-        <v>379</v>
+        <v>422</v>
       </c>
       <c r="Q8" t="s">
-        <v>387</v>
+        <v>262</v>
       </c>
       <c r="S8" t="s">
-        <v>498</v>
-      </c>
-      <c r="T8" t="s">
-        <v>505</v>
+        <v>270</v>
       </c>
       <c r="U8" t="s">
-        <v>520</v>
+        <v>381</v>
+      </c>
+      <c r="V8" t="s">
+        <v>388</v>
+      </c>
+      <c r="W8" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>205</v>
+        <v>88</v>
       </c>
       <c r="E9" t="s">
-        <v>237</v>
+        <v>120</v>
       </c>
       <c r="I9" t="s">
-        <v>332</v>
+        <v>215</v>
       </c>
       <c r="K9" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="M9" t="s">
-        <v>348</v>
+        <v>231</v>
       </c>
       <c r="N9" t="s">
-        <v>360</v>
+        <v>243</v>
       </c>
       <c r="P9" t="s">
-        <v>380</v>
+        <v>423</v>
       </c>
       <c r="Q9" t="s">
-        <v>388</v>
-      </c>
-      <c r="T9" t="s">
-        <v>506</v>
-      </c>
-      <c r="U9" t="s">
-        <v>521</v>
+        <v>263</v>
+      </c>
+      <c r="S9" t="s">
+        <v>271</v>
+      </c>
+      <c r="V9" t="s">
+        <v>389</v>
+      </c>
+      <c r="W9" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>183</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>206</v>
+        <v>89</v>
       </c>
       <c r="E10" t="s">
-        <v>238</v>
+        <v>121</v>
       </c>
       <c r="I10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="K10" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="M10" t="s">
-        <v>349</v>
+        <v>232</v>
       </c>
       <c r="N10" t="s">
-        <v>361</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>389</v>
-      </c>
-      <c r="T10" t="s">
-        <v>507</v>
-      </c>
-      <c r="U10" t="s">
-        <v>522</v>
+        <v>244</v>
+      </c>
+      <c r="P10" t="s">
+        <v>424</v>
+      </c>
+      <c r="S10" t="s">
+        <v>272</v>
+      </c>
+      <c r="V10" t="s">
+        <v>390</v>
+      </c>
+      <c r="W10" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>207</v>
+        <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>239</v>
+        <v>122</v>
       </c>
       <c r="I11" t="s">
-        <v>103</v>
+        <v>45</v>
       </c>
       <c r="K11" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
       <c r="M11" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="N11" t="s">
-        <v>362</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>390</v>
-      </c>
-      <c r="T11" t="s">
-        <v>508</v>
-      </c>
-      <c r="U11" t="s">
-        <v>523</v>
+        <v>245</v>
+      </c>
+      <c r="S11" t="s">
+        <v>273</v>
+      </c>
+      <c r="V11" t="s">
+        <v>391</v>
+      </c>
+      <c r="W11" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>184</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>240</v>
+        <v>123</v>
       </c>
       <c r="I12" t="s">
-        <v>333</v>
+        <v>216</v>
       </c>
       <c r="M12" t="s">
-        <v>350</v>
+        <v>233</v>
       </c>
       <c r="N12" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>391</v>
-      </c>
-      <c r="T12" t="s">
-        <v>509</v>
+        <v>246</v>
+      </c>
+      <c r="S12" t="s">
+        <v>274</v>
+      </c>
+      <c r="V12" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>185</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>208</v>
+        <v>91</v>
       </c>
       <c r="E13" t="s">
-        <v>241</v>
+        <v>124</v>
       </c>
       <c r="I13" t="s">
-        <v>334</v>
+        <v>217</v>
       </c>
       <c r="M13" t="s">
-        <v>351</v>
+        <v>234</v>
       </c>
       <c r="N13" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>392</v>
-      </c>
-      <c r="T13" t="s">
-        <v>510</v>
+        <v>247</v>
+      </c>
+      <c r="S13" t="s">
+        <v>275</v>
+      </c>
+      <c r="V13" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>186</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>209</v>
+        <v>92</v>
       </c>
       <c r="E14" t="s">
-        <v>242</v>
+        <v>125</v>
       </c>
       <c r="I14" t="s">
-        <v>335</v>
+        <v>218</v>
       </c>
       <c r="M14" t="s">
-        <v>352</v>
+        <v>235</v>
       </c>
       <c r="N14" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>393</v>
-      </c>
-      <c r="T14" t="s">
-        <v>511</v>
+        <v>248</v>
+      </c>
+      <c r="S14" t="s">
+        <v>276</v>
+      </c>
+      <c r="V14" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>187</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>210</v>
+        <v>93</v>
       </c>
       <c r="E15" t="s">
-        <v>243</v>
+        <v>126</v>
       </c>
       <c r="I15" t="s">
-        <v>336</v>
+        <v>219</v>
       </c>
       <c r="N15" t="s">
-        <v>366</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>394</v>
-      </c>
-      <c r="T15" t="s">
-        <v>512</v>
+        <v>249</v>
+      </c>
+      <c r="S15" t="s">
+        <v>277</v>
+      </c>
+      <c r="V15" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>188</v>
+        <v>411</v>
       </c>
       <c r="C16" t="s">
-        <v>211</v>
+        <v>94</v>
       </c>
       <c r="E16" t="s">
-        <v>244</v>
+        <v>127</v>
       </c>
       <c r="I16" t="s">
-        <v>337</v>
+        <v>220</v>
       </c>
       <c r="N16" t="s">
-        <v>367</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>395</v>
-      </c>
-      <c r="T16" t="s">
-        <v>513</v>
+        <v>250</v>
+      </c>
+      <c r="S16" t="s">
+        <v>278</v>
+      </c>
+      <c r="V16" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>189</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>95</v>
       </c>
       <c r="E17" t="s">
-        <v>245</v>
+        <v>128</v>
       </c>
       <c r="I17" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>396</v>
+        <v>47</v>
+      </c>
+      <c r="S17" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>190</v>
+        <v>412</v>
       </c>
       <c r="C18" t="s">
-        <v>213</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>246</v>
+        <v>129</v>
       </c>
       <c r="I18" t="s">
-        <v>338</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>397</v>
+        <v>221</v>
+      </c>
+      <c r="S18" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>191</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>214</v>
+        <v>97</v>
       </c>
       <c r="E19" t="s">
-        <v>247</v>
+        <v>130</v>
       </c>
       <c r="I19" t="s">
-        <v>339</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>398</v>
+        <v>222</v>
+      </c>
+      <c r="S19" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>192</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>215</v>
+        <v>98</v>
       </c>
       <c r="E20" t="s">
-        <v>248</v>
+        <v>131</v>
       </c>
       <c r="I20" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>399</v>
+        <v>48</v>
+      </c>
+      <c r="S20" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>216</v>
+        <v>99</v>
       </c>
       <c r="E21" t="s">
-        <v>249</v>
+        <v>132</v>
       </c>
       <c r="I21" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>400</v>
+        <v>49</v>
+      </c>
+      <c r="S21" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="22">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
       <c r="C22" t="s">
-        <v>217</v>
+        <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>250</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>401</v>
+        <v>133</v>
+      </c>
+      <c r="S22" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="23">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
       <c r="C23" t="s">
-        <v>218</v>
+        <v>101</v>
       </c>
       <c r="E23" t="s">
-        <v>251</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>402</v>
+        <v>134</v>
+      </c>
+      <c r="S23" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="24">
       <c r="C24" t="s">
-        <v>219</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>252</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>403</v>
+        <v>135</v>
+      </c>
+      <c r="S24" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="25">
       <c r="C25" t="s">
-        <v>220</v>
+        <v>103</v>
       </c>
       <c r="E25" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>404</v>
+        <v>136</v>
+      </c>
+      <c r="S25" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="26">
       <c r="C26" t="s">
-        <v>221</v>
+        <v>104</v>
       </c>
       <c r="E26" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>405</v>
+        <v>137</v>
+      </c>
+      <c r="S26" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="27">
       <c r="C27" t="s">
-        <v>222</v>
+        <v>105</v>
       </c>
       <c r="E27" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>406</v>
+        <v>138</v>
+      </c>
+      <c r="S27" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="28">
       <c r="C28" t="s">
-        <v>223</v>
+        <v>106</v>
       </c>
       <c r="E28" t="s">
-        <v>256</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>407</v>
+        <v>139</v>
+      </c>
+      <c r="S28" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="29">
       <c r="C29" t="s">
-        <v>224</v>
+        <v>107</v>
       </c>
       <c r="E29" t="s">
-        <v>257</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>408</v>
+        <v>140</v>
+      </c>
+      <c r="S29" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="30">
       <c r="C30" t="s">
-        <v>225</v>
+        <v>108</v>
       </c>
       <c r="E30" t="s">
-        <v>258</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>409</v>
+        <v>141</v>
+      </c>
+      <c r="S30" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="31">
       <c r="C31" t="s">
-        <v>226</v>
+        <v>109</v>
       </c>
       <c r="E31" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>410</v>
+        <v>142</v>
+      </c>
+      <c r="S31" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="32">
       <c r="E32" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>411</v>
+        <v>143</v>
+      </c>
+      <c r="S32" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="33">
       <c r="E33" t="s">
-        <v>261</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>412</v>
+        <v>144</v>
+      </c>
+      <c r="S33" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="34">
       <c r="E34" t="s">
-        <v>262</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>413</v>
+        <v>145</v>
+      </c>
+      <c r="S34" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="35">
       <c r="E35" t="s">
-        <v>263</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>414</v>
+        <v>146</v>
+      </c>
+      <c r="S35" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="36">
       <c r="E36" t="s">
-        <v>264</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>415</v>
+        <v>147</v>
+      </c>
+      <c r="S36" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="37">
       <c r="E37" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>416</v>
+        <v>148</v>
+      </c>
+      <c r="S37" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="38">
       <c r="E38" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>417</v>
+        <v>149</v>
+      </c>
+      <c r="S38" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="39">
       <c r="E39" t="s">
-        <v>267</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>418</v>
+        <v>150</v>
+      </c>
+      <c r="S39" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="40">
       <c r="E40" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>419</v>
+        <v>151</v>
+      </c>
+      <c r="S40" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="41">
       <c r="E41" t="s">
-        <v>269</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>420</v>
+        <v>152</v>
+      </c>
+      <c r="S41" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="42">
       <c r="E42" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>421</v>
+        <v>153</v>
+      </c>
+      <c r="S42" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="43">
       <c r="E43" t="s">
-        <v>271</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>422</v>
+        <v>154</v>
+      </c>
+      <c r="S43" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="44">
       <c r="E44" t="s">
-        <v>272</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>423</v>
+        <v>155</v>
+      </c>
+      <c r="S44" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="45">
       <c r="E45" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>424</v>
+        <v>156</v>
+      </c>
+      <c r="S45" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="46">
       <c r="E46" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>425</v>
+        <v>157</v>
+      </c>
+      <c r="S46" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="47">
       <c r="E47" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>426</v>
+        <v>158</v>
+      </c>
+      <c r="S47" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="48">
       <c r="E48" t="s">
-        <v>276</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>427</v>
+        <v>159</v>
+      </c>
+      <c r="S48" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="49">
       <c r="E49" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>428</v>
+        <v>160</v>
+      </c>
+      <c r="S49" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="50">
       <c r="E50" t="s">
-        <v>278</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>429</v>
+        <v>161</v>
+      </c>
+      <c r="S50" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="51">
       <c r="E51" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>430</v>
+        <v>162</v>
+      </c>
+      <c r="S51" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="52">
       <c r="E52" t="s">
-        <v>280</v>
-      </c>
-      <c r="Q52" t="s">
-        <v>431</v>
+        <v>165</v>
+      </c>
+      <c r="S52" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="53">
       <c r="E53" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>432</v>
+        <v>166</v>
+      </c>
+      <c r="S53" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="54">
       <c r="E54" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>433</v>
+        <v>167</v>
+      </c>
+      <c r="S54" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="55">
       <c r="E55" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>434</v>
+        <v>168</v>
+      </c>
+      <c r="S55" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="56">
       <c r="E56" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>435</v>
+        <v>169</v>
+      </c>
+      <c r="S56" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="57">
       <c r="E57" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>436</v>
+        <v>170</v>
+      </c>
+      <c r="S57" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="58">
       <c r="E58" t="s">
-        <v>286</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>437</v>
+        <v>171</v>
+      </c>
+      <c r="S58" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="59">
       <c r="E59" t="s">
-        <v>287</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>438</v>
+        <v>172</v>
+      </c>
+      <c r="S59" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="60">
       <c r="E60" t="s">
-        <v>288</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>439</v>
+        <v>173</v>
+      </c>
+      <c r="S60" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="61">
       <c r="E61" t="s">
-        <v>289</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>440</v>
+        <v>174</v>
+      </c>
+      <c r="S61" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="62">
       <c r="E62" t="s">
-        <v>290</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>441</v>
+        <v>175</v>
+      </c>
+      <c r="S62" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="63">
       <c r="E63" t="s">
-        <v>291</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>442</v>
+        <v>176</v>
+      </c>
+      <c r="S63" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="64">
       <c r="E64" t="s">
-        <v>292</v>
-      </c>
-      <c r="Q64" t="s">
-        <v>443</v>
+        <v>177</v>
+      </c>
+      <c r="S64" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="65">
       <c r="E65" t="s">
-        <v>293</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>444</v>
+        <v>178</v>
+      </c>
+      <c r="S65" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="66">
       <c r="E66" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>445</v>
+        <v>179</v>
+      </c>
+      <c r="S66" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="67">
       <c r="E67" t="s">
-        <v>295</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>446</v>
+        <v>180</v>
+      </c>
+      <c r="S67" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="68">
       <c r="E68" t="s">
-        <v>296</v>
-      </c>
-      <c r="Q68" t="s">
-        <v>447</v>
+        <v>181</v>
+      </c>
+      <c r="S68" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="69">
       <c r="E69" t="s">
-        <v>297</v>
-      </c>
-      <c r="Q69" t="s">
-        <v>448</v>
+        <v>413</v>
+      </c>
+      <c r="S69" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="70">
       <c r="E70" t="s">
-        <v>298</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>449</v>
+        <v>182</v>
+      </c>
+      <c r="S70" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="71">
       <c r="E71" t="s">
-        <v>299</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>450</v>
+        <v>414</v>
+      </c>
+      <c r="S71" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="72">
       <c r="E72" t="s">
-        <v>300</v>
-      </c>
-      <c r="Q72" t="s">
-        <v>451</v>
+        <v>183</v>
+      </c>
+      <c r="S72" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="73">
       <c r="E73" t="s">
-        <v>301</v>
-      </c>
-      <c r="Q73" t="s">
-        <v>452</v>
+        <v>184</v>
+      </c>
+      <c r="S73" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="74">
       <c r="E74" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q74" t="s">
-        <v>453</v>
+        <v>185</v>
+      </c>
+      <c r="S74" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="75">
       <c r="E75" t="s">
-        <v>303</v>
-      </c>
-      <c r="Q75" t="s">
-        <v>454</v>
+        <v>186</v>
+      </c>
+      <c r="S75" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="76">
       <c r="E76" t="s">
-        <v>304</v>
-      </c>
-      <c r="Q76" t="s">
-        <v>455</v>
+        <v>187</v>
+      </c>
+      <c r="S76" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="77">
       <c r="E77" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q77" t="s">
-        <v>456</v>
+        <v>188</v>
+      </c>
+      <c r="S77" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="78">
       <c r="E78" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q78" t="s">
-        <v>457</v>
+        <v>189</v>
+      </c>
+      <c r="S78" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="79">
       <c r="E79" t="s">
-        <v>307</v>
-      </c>
-      <c r="Q79" t="s">
-        <v>458</v>
+        <v>190</v>
+      </c>
+      <c r="S79" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="80">
       <c r="E80" t="s">
-        <v>308</v>
-      </c>
-      <c r="Q80" t="s">
-        <v>459</v>
+        <v>191</v>
+      </c>
+      <c r="S80" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="81">
       <c r="E81" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q81" t="s">
-        <v>460</v>
+        <v>192</v>
+      </c>
+      <c r="S81" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="82">
       <c r="E82" t="s">
-        <v>310</v>
-      </c>
-      <c r="Q82" t="s">
-        <v>461</v>
+        <v>193</v>
+      </c>
+      <c r="S82" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="83">
       <c r="E83" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q83" t="s">
-        <v>462</v>
+        <v>194</v>
+      </c>
+      <c r="S83" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="84">
       <c r="E84" t="s">
-        <v>312</v>
-      </c>
-      <c r="Q84" t="s">
-        <v>463</v>
+        <v>195</v>
+      </c>
+      <c r="S84" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="85">
       <c r="E85" t="s">
-        <v>313</v>
-      </c>
-      <c r="Q85" t="s">
-        <v>464</v>
+        <v>196</v>
+      </c>
+      <c r="S85" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="86">
       <c r="E86" t="s">
-        <v>314</v>
-      </c>
-      <c r="Q86" t="s">
-        <v>465</v>
+        <v>197</v>
+      </c>
+      <c r="S86" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="87">
       <c r="E87" t="s">
-        <v>315</v>
-      </c>
-      <c r="Q87" t="s">
-        <v>466</v>
+        <v>198</v>
+      </c>
+      <c r="S87" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="88">
       <c r="E88" t="s">
-        <v>316</v>
-      </c>
-      <c r="Q88" t="s">
-        <v>467</v>
+        <v>199</v>
+      </c>
+      <c r="S88" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="89">
       <c r="E89" t="s">
-        <v>317</v>
-      </c>
-      <c r="Q89" t="s">
-        <v>468</v>
+        <v>200</v>
+      </c>
+      <c r="S89" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="90">
       <c r="E90" t="s">
-        <v>318</v>
-      </c>
-      <c r="Q90" t="s">
-        <v>469</v>
+        <v>201</v>
+      </c>
+      <c r="S90" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="91">
       <c r="E91" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q91" t="s">
-        <v>470</v>
+        <v>202</v>
+      </c>
+      <c r="S91" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="92">
-      <c r="Q92" t="s">
-        <v>471</v>
+      <c r="S92" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="93">
-      <c r="Q93" t="s">
-        <v>472</v>
+      <c r="S93" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="94">
-      <c r="Q94" t="s">
-        <v>473</v>
+      <c r="S94" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="95">
-      <c r="Q95" t="s">
-        <v>474</v>
+      <c r="S95" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="96">
-      <c r="Q96" t="s">
-        <v>475</v>
+      <c r="S96" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="97">
-      <c r="Q97" t="s">
-        <v>476</v>
+      <c r="S97" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="98">
-      <c r="Q98" t="s">
-        <v>477</v>
+      <c r="S98" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="99">
-      <c r="Q99" t="s">
-        <v>478</v>
+      <c r="S99" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="100">
-      <c r="Q100" t="s">
-        <v>479</v>
+      <c r="S100" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="101">
-      <c r="Q101" t="s">
-        <v>480</v>
+      <c r="S101" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="102">
-      <c r="Q102" t="s">
-        <v>481</v>
+      <c r="S102" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="103">
-      <c r="Q103" t="s">
-        <v>482</v>
+      <c r="S103" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="104">
-      <c r="Q104" t="s">
-        <v>145</v>
+      <c r="S104" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="105">
-      <c r="Q105" t="s">
-        <v>483</v>
+      <c r="S105" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="106">
-      <c r="Q106" t="s">
-        <v>484</v>
+      <c r="S106" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="107">
-      <c r="Q107" t="s">
-        <v>485</v>
+      <c r="S107" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="108">
-      <c r="Q108" t="s">
-        <v>486</v>
+      <c r="S108" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4582,11 +3917,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P697"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="true" workbookViewId="0" zoomScale="100">
+      <selection sqref="A5" activeCell="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4606,31 +3941,31 @@
   </cols>
   <sheetData>
     <row customHeight="1" ht="23" r="1" spans="1:15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="31"/>
       <c r="E1" s="24" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>0</v>
+        <v>409</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>1</v>
+        <v>410</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M1" s="25"/>
       <c r="N1" s="25"/>
@@ -4638,27 +3973,27 @@
     </row>
     <row customHeight="1" ht="140" r="2" spans="1:15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>176</v>
+        <v>59</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
       <c r="D2" s="34"/>
       <c r="E2" s="21" t="s">
-        <v>179</v>
+        <v>62</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>177</v>
+        <v>60</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="23"/>
       <c r="I2" s="22" t="s">
-        <v>180</v>
+        <v>63</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="30"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="28"/>
       <c r="O2" s="4"/>
     </row>
     <row customHeight="1" ht="10" r="3" spans="1:15" thickBot="1" x14ac:dyDescent="0.25">
@@ -4680,67 +4015,67 @@
     </row>
     <row customFormat="1" customHeight="1" ht="20" r="4" s="7" spans="1:15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>524</v>
+        <v>407</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>408</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>525</v>
-      </c>
-      <c r="D4" s="24" t="s">
+      <c r="E4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="I4" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>178</v>
+        <v>61</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row customHeight="1" ht="22" r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>147</v>
+        <v>51</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>148</v>
+        <v>52</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>172</v>
+        <v>55</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>173</v>
+        <v>56</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
@@ -4755,19 +4090,19 @@
     <row customHeight="1" ht="22" r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="6" t="s">
-        <v>149</v>
+        <v>53</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>174</v>
+        <v>57</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>175</v>
+        <v>58</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -15767,10 +15102,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D5:D698" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D5:D698" type="list" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C5" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C5" type="list" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>target</formula1>
     </dataValidation>
   </dataValidations>
@@ -15778,7 +15113,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>'#system'!$A$2:$A$50</xm:f>
           </x14:formula1>

</xml_diff>